<commit_message>
add check for non-unqiue name entry and halt sign-in if so
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>On Time</t>
   </si>
@@ -37,18 +34,6 @@
     <t>Part</t>
   </si>
   <si>
-    <t>Member 1</t>
-  </si>
-  <si>
-    <t>Member 2</t>
-  </si>
-  <si>
-    <t>Member 3</t>
-  </si>
-  <si>
-    <t>Member 4</t>
-  </si>
-  <si>
     <t>Rehearsal Start Time</t>
   </si>
   <si>
@@ -64,18 +49,6 @@
     <t>B2</t>
   </si>
   <si>
-    <t>Member 5</t>
-  </si>
-  <si>
-    <t>Member 6</t>
-  </si>
-  <si>
-    <t>Member 7</t>
-  </si>
-  <si>
-    <t>Member 8</t>
-  </si>
-  <si>
     <t>abc123</t>
   </si>
   <si>
@@ -104,6 +77,39 @@
   </si>
   <si>
     <t>Scan ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>Six</t>
+  </si>
+  <si>
+    <t>Seven</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Person</t>
   </si>
 </sst>
 </file>
@@ -424,47 +430,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -473,122 +483,147 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E5">
+        <v>123457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>123457</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7">
+        <v>123458</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>123459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="D7">
-        <v>123458</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>123460</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>123461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8">
-        <v>123459</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10">
-        <v>123460</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11">
-        <v>123461</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="E13">
+        <v>123462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>123462</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14">
+      <c r="E14">
         <v>123463</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add ID check for last and full name, update getName() to handle numeric and blank cell values
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -145,8 +145,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,7 +436,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,17 +476,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>